<commit_message>
fix: update single binary file
Update composer.json
</commit_message>
<xml_diff>
--- a/stubs/source/demo1.xlsx
+++ b/stubs/source/demo1.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrohmani/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrohmani/Project/stech/packages/excel-joiner/stubs/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B305301-F4E4-2848-BC9C-2C41D73E5494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7205FF3A-521E-134F-B98C-5384B87ECC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" xr2:uid="{045B195E-BC39-8E44-BF36-283762D25AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,16 +36,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>DEMO1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Order ID</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>Keyboard</t>
+  </si>
+  <si>
+    <t>Bob Johnson</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Alice Brown</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>Sales Order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -53,16 +92,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,12 +123,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,15 +462,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D622355-C571-CA44-8E44-E214AEB89C49}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>1001</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>1002</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>1003</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>1004</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>